<commit_message>
DeCamino version found under salva pc folder
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agostino\Documents\Visual Studio 2012\Projects\MiPaladar DKM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8925"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="15600" windowHeight="8925"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>*CUC y CUP, EUR, USD</t>
   </si>
@@ -81,9 +86,6 @@
     <t>buscar transaccion</t>
   </si>
   <si>
-    <t>filtrar por tipo de trans en follow product</t>
-  </si>
-  <si>
     <t>consulta muy largas en otro hilo??</t>
   </si>
   <si>
@@ -138,9 +140,6 @@
     <t>guardar y eliminar en background</t>
   </si>
   <si>
-    <t>cambiar producción a trabajo con parte izquierda y derecha</t>
-  </si>
-  <si>
     <t>quitar propiedades: compras, ingrediente, entrante</t>
   </si>
   <si>
@@ -156,9 +155,6 @@
     <t>fondo y descuento configurable</t>
   </si>
   <si>
-    <t>Ventas</t>
-  </si>
-  <si>
     <t>Compras</t>
   </si>
   <si>
@@ -174,27 +170,15 @@
     <t>poder cancelar marcha, pero no eliminar del todo</t>
   </si>
   <si>
-    <t>unit testing, dependency injection, repository pattern</t>
-  </si>
-  <si>
-    <t>datos de prueba, base de datos inicial</t>
-  </si>
-  <si>
     <t>Contabilidad</t>
   </si>
   <si>
-    <t>cargar reportes sin realmente crear la venta</t>
-  </si>
-  <si>
     <t>cuenta casa</t>
   </si>
   <si>
     <t>inplace autocomplete</t>
   </si>
   <si>
-    <t>organizar el inventario, definir tipos de productos</t>
-  </si>
-  <si>
     <t>vista previa a la hora de imprimir, poder configurar proceso la impresión</t>
   </si>
   <si>
@@ -210,26 +194,95 @@
     <t>Quorion</t>
   </si>
   <si>
-    <t>Pa cuando no haya mas na q hacer</t>
-  </si>
-  <si>
-    <t>categorías de inventario/venta, con subcategorías y eqiquetas</t>
-  </si>
-  <si>
-    <t>distinguir entre alimentos, bebidas, cigarros, insumos, etc.</t>
-  </si>
-  <si>
-    <t>usar qdll a full, procesar otros tipos de reportes (101)</t>
-  </si>
-  <si>
-    <t>mas opciones a la hora de escoger fechas (hoy, semana, mes, custom)</t>
+    <t>recetas complejas, una receta q contenga otra receta, reconocer ciclos</t>
+  </si>
+  <si>
+    <t>poder especificar recetas para mas de una porcion</t>
+  </si>
+  <si>
+    <t>mas opciones a la hora de escoger fechas (hoy, semana, mes, específico)</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>ultimos 7 dias</t>
+  </si>
+  <si>
+    <t>analizar condiciones en las que hay que actualizar los outgredients</t>
+  </si>
+  <si>
+    <t>categorías de inventario, con subcategorías y etiquetas</t>
+  </si>
+  <si>
+    <t>arreglar costos de productos q están mal en el inventario</t>
+  </si>
+  <si>
+    <t>treeview expand, collapse, isexpanded</t>
+  </si>
+  <si>
+    <t>exportar a excel, arreglar comando</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>arreglar Roles y Permisos</t>
+  </si>
+  <si>
+    <t>cargar carpeta completa</t>
+  </si>
+  <si>
+    <t>cargar reporte plu sin realmente crear la venta</t>
+  </si>
+  <si>
+    <t>procesar reporte 103, halar vales por separado</t>
+  </si>
+  <si>
+    <t>top dependientes, indices, bottom products</t>
+  </si>
+  <si>
+    <t>exportar a excel nuevos reportes</t>
+  </si>
+  <si>
+    <t>reportes de proyecciones</t>
+  </si>
+  <si>
+    <t>terminar eliminar Rol</t>
+  </si>
+  <si>
+    <t>treelistview</t>
+  </si>
+  <si>
+    <t>Miscelaneas, Ranking &amp; Indices</t>
+  </si>
+  <si>
+    <t>Save Reports</t>
+  </si>
+  <si>
+    <t>iconos, imagenes, pacotilla</t>
+  </si>
+  <si>
+    <t>importar-exportar</t>
+  </si>
+  <si>
+    <t>boton eliminar en ingredientes, lineitems</t>
+  </si>
+  <si>
+    <t>merge product</t>
+  </si>
+  <si>
+    <t>unit testing, dependency injection</t>
+  </si>
+  <si>
+    <t>base de datos inicial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +343,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -340,14 +406,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -623,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -631,15 +697,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.85546875" customWidth="1"/>
+    <col min="1" max="1" width="53.28515625" customWidth="1"/>
     <col min="2" max="2" width="72.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -653,280 +719,329 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>41</v>
+      <c r="A3" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
+      <c r="B13" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" t="s">
-        <v>26</v>
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>6</v>
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>49</v>
+      <c r="A27" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>21</v>
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>53</v>
+      <c r="A30" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>1</v>
+      <c r="B38" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>18</v>
+      <c r="A39" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="8"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>38</v>
+      <c r="A41" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>52</v>
+      <c r="A42" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -935,58 +1050,64 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
+      <c r="A47" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="8"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
+      <c r="A67" s="6"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+    </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
+      <c r="A76" s="1"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>